<commit_message>
changes in plotting functions. IN/OUT now more homogeneous
</commit_message>
<xml_diff>
--- a/Paleointensity/statistics check.xlsx
+++ b/Paleointensity/statistics check.xlsx
@@ -987,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1883,7 +1883,7 @@
         <v>2.8611239216326641E-20</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19:D19" si="8">(C2-S$3)^2</f>
+        <f t="shared" ref="C19" si="8">(C2-S$3)^2</f>
         <v>3.3073437090477124E-18</v>
       </c>
       <c r="D19" s="1">
@@ -1910,8 +1910,8 @@
         <v>1.6596259758918569E-16</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="9"/>
-        <v>1.7134678742392859E-16</v>
+        <f>(E2-U$3)*(O2-U$2)</f>
+        <v>-9.6306767224444423E-17</v>
       </c>
       <c r="K19">
         <v>20</v>
@@ -1938,11 +1938,11 @@
         <v>300</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" ref="B20:B33" si="11">(B3-R$3)^2</f>
+        <f t="shared" ref="B20:B32" si="11">(B3-R$3)^2</f>
         <v>6.8566443664489824E-19</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ref="C20:E33" si="12">(C3-S$3)^2</f>
+        <f t="shared" ref="C20:E32" si="12">(C3-S$3)^2</f>
         <v>2.479082932229141E-18</v>
       </c>
       <c r="D20" s="1">
@@ -1957,7 +1957,7 @@
         <v>300</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G33" si="13">(B3-R$3)*(G3-R$2)</f>
+        <f t="shared" ref="G20:G32" si="13">(B3-R$3)*(G3-R$2)</f>
         <v>1.65671877074898E-18</v>
       </c>
       <c r="H20" s="1">
@@ -1969,26 +1969,26 @@
         <v>1.5685882115204289E-16</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="9"/>
-        <v>1.6226327918812144E-16</v>
+        <f t="shared" ref="J20:J33" si="14">(E3-U$3)*(O3-U$2)</f>
+        <v>-8.8422044729448336E-17</v>
       </c>
       <c r="K20">
         <v>300</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" ref="L20:L32" si="14">(L3-R$2)^2</f>
+        <f t="shared" ref="L20:L32" si="15">(L3-R$2)^2</f>
         <v>5.3754753714796E-20</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" ref="M20:M32" si="15">(M3-S$2)^2</f>
+        <f t="shared" ref="M20:M32" si="16">(M3-S$2)^2</f>
         <v>2.969503243602611E-18</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" ref="N20:O32" si="16">(N3-T$2)^2</f>
+        <f t="shared" ref="N20:O32" si="17">(N3-T$2)^2</f>
         <v>7.677782618458977E-17</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.8944397127643026E-17</v>
       </c>
     </row>
@@ -2005,11 +2005,11 @@
         <v>2.4913793231819981E-18</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" ref="D21:E33" si="17">(D4-T$3)^2</f>
+        <f t="shared" ref="D21:E32" si="18">(D4-T$3)^2</f>
         <v>8.1351560640100001E-17</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.4283742183778773E-17</v>
       </c>
       <c r="F21">
@@ -2028,26 +2028,26 @@
         <v>1.3998914751204286E-16</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="9"/>
-        <v>1.448193435958285E-16</v>
+        <f t="shared" si="14"/>
+        <v>-7.9361304156909575E-17</v>
       </c>
       <c r="K21">
         <v>450</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8.8463295885765318E-19</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.2058923034026129E-18</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.1847589036018348E-17</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.4726352132685285E-17</v>
       </c>
     </row>
@@ -2064,11 +2064,11 @@
         <v>1.5760552186248562E-18</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.3258321320099978E-17</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.5080417744164271E-17</v>
       </c>
       <c r="F22">
@@ -2087,26 +2087,26 @@
         <v>1.193718796234714E-16</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="9"/>
-        <v>1.2294682936596933E-16</v>
+        <f t="shared" si="14"/>
+        <v>-6.5064575586961478E-17</v>
       </c>
       <c r="K22">
         <v>490</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.993342471479596E-20</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.2886384648711849E-18</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.2762769384589778E-17</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.5048737286125224E-17</v>
       </c>
     </row>
@@ -2123,11 +2123,11 @@
         <v>1.0535182652391414E-18</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.2265814840100025E-17</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.360172840911556E-17</v>
       </c>
       <c r="F23">
@@ -2146,26 +2146,26 @@
         <v>1.0698738062061431E-16</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="9"/>
-        <v>1.1007190131541477E-16</v>
+        <f t="shared" si="14"/>
+        <v>-5.5094218394991728E-17</v>
       </c>
       <c r="K23">
         <v>500</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.3589615671479563E-19</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2928250871940403E-18</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.4882845390304109E-17</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.662826536837657E-17</v>
       </c>
     </row>
@@ -2182,11 +2182,11 @@
         <v>5.7019168382628466E-19</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.5733201580100009E-17</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.6170762029427732E-17</v>
       </c>
       <c r="F24">
@@ -2205,26 +2205,26 @@
         <v>5.0968480546328586E-17</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="9"/>
-        <v>5.2502403516657762E-17</v>
+        <f t="shared" si="14"/>
+        <v>-2.4945916035154835E-17</v>
       </c>
       <c r="K24">
         <v>510</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.6214361857653078E-20</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.6132166628268971E-18</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3.7140440253161234E-17</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3.8482956195912654E-17</v>
       </c>
     </row>
@@ -2241,11 +2241,11 @@
         <v>2.5473256623771385E-19</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3671580200100002E-17</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3975560189465647E-17</v>
       </c>
       <c r="F25">
@@ -2264,26 +2264,26 @@
         <v>5.0728743793471436E-17</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="9"/>
-        <v>5.2172501844418597E-17</v>
+        <f t="shared" si="14"/>
+        <v>-1.8769726031162951E-17</v>
       </c>
       <c r="K25">
         <v>515</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3856953071479579E-19</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.2609586862118341E-19</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.4554955616018364E-17</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.5208478981076631E-17</v>
       </c>
     </row>
@@ -2300,11 +2300,11 @@
         <v>3.5122649996285793E-20</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.0981812201000035E-18</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.1629353978239382E-18</v>
       </c>
       <c r="F26">
@@ -2323,26 +2323,26 @@
         <v>2.0190352544900018E-17</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="9"/>
-        <v>2.0855759629680333E-17</v>
+        <f t="shared" si="14"/>
+        <v>-3.7180076350803382E-18</v>
       </c>
       <c r="K26">
         <v>520</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.6204592742908166E-19</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0984230809689831E-19</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.1866399703040827E-18</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.3911205061525009E-18</v>
       </c>
     </row>
@@ -2359,11 +2359,11 @@
         <v>5.5314158027715111E-20</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.191850640099999E-18</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.2946279092476272E-18</v>
       </c>
       <c r="F27">
@@ -2382,26 +2382,26 @@
         <v>-2.0340014307957142E-17</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="9"/>
-        <v>-2.1181018899847803E-17</v>
+        <f t="shared" si="14"/>
+        <v>-3.9264215852031262E-19</v>
       </c>
       <c r="K27">
         <v>525</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.4282297685765294E-19</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.3487009668984189E-21</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.8420961732654121E-20</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.7186433158149618E-20</v>
       </c>
     </row>
@@ -2418,11 +2418,11 @@
         <v>4.7940338786200161E-19</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.2245277920099996E-17</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.2761865305068338E-17</v>
       </c>
       <c r="F28">
@@ -2441,26 +2441,26 @@
         <v>-6.7463278226528572E-17</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="9"/>
-        <v>-6.9307650917854901E-17</v>
+        <f t="shared" si="14"/>
+        <v>-1.9368559209287754E-17</v>
       </c>
       <c r="K28">
         <v>530</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7043745537193876E-19</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2501551802547027E-19</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.6343457941732661E-17</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.6481122298889693E-17</v>
       </c>
     </row>
@@ -2477,11 +2477,11 @@
         <v>1.6335130804034316E-18</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.2168253136099979E-17</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.3935342179972393E-17</v>
       </c>
       <c r="F29">
@@ -2500,26 +2500,26 @@
         <v>-1.2912437585095714E-16</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="9"/>
-        <v>-1.3332796701293636E-16</v>
+        <f t="shared" si="14"/>
+        <v>-7.6235871915021254E-17</v>
       </c>
       <c r="K29">
         <v>535</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.0995903371479589E-19</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.5955637373469013E-18</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.5993137480589799E-17</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.860798361487608E-17</v>
       </c>
     </row>
@@ -2536,11 +2536,11 @@
         <v>2.730259271435146E-18</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2071175187209997E-16</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2345771256462142E-16</v>
       </c>
       <c r="F30">
@@ -2559,26 +2559,26 @@
         <v>-1.7519369895967141E-16</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="9"/>
-        <v>-1.8081893930133737E-16</v>
+        <f t="shared" si="14"/>
+        <v>-1.3496169811174676E-16</v>
       </c>
       <c r="K30">
         <v>540</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.7851875000510238E-20</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.9552333158486125E-18</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.4292451848230406E-16</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.4753764328552726E-16</v>
       </c>
     </row>
@@ -2595,11 +2595,11 @@
         <v>4.940526969976004E-18</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7381759232009997E-16</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7954015545198348E-16</v>
       </c>
       <c r="F31">
@@ -2618,26 +2618,26 @@
         <v>-2.1320758758581429E-16</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="9"/>
-        <v>-2.2041208555597249E-16</v>
+        <f t="shared" si="14"/>
+        <v>-1.9577045340141296E-16</v>
       </c>
       <c r="K31">
         <v>545</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.5013696797193877E-19</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.1658617704594699E-18</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.0673275848173274E-16</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.1346795834341798E-16</v>
       </c>
     </row>
@@ -2654,11 +2654,11 @@
         <v>6.8635350155366544E-18</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.1097649650089997E-16</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.1858863908731433E-16</v>
       </c>
       <c r="F32">
@@ -2677,26 +2677,26 @@
         <v>-2.3716039458112854E-16</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="9"/>
-        <v>-2.457083234774212E-16</v>
+        <f t="shared" si="14"/>
+        <v>-2.3900277031568314E-16</v>
       </c>
       <c r="K32">
         <v>550</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.40153431714796E-19</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.4035488092615498E-18</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.5202338113110405E-16</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2.6132339016829643E-16</v>
       </c>
     </row>
@@ -2709,15 +2709,15 @@
         <v>4.3632816725714284E-18</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" ref="C33" si="18">SUM(C19:C32)</f>
+        <f t="shared" ref="C33" si="19">SUM(C19:C32)</f>
         <v>2.8469978231624087E-17</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" ref="D33:E33" si="19">SUM(D19:D32)</f>
+        <f t="shared" ref="D33:E33" si="20">SUM(D19:D32)</f>
         <v>1.0320681481501998E-15</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.0636373756204745E-15</v>
       </c>
       <c r="F33" t="s">
@@ -2728,16 +2728,16 @@
         <v>1.4165454241857166E-18</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" ref="H33" si="20">SUM(H19:H32)</f>
+        <f t="shared" ref="H33" si="21">SUM(H19:H32)</f>
         <v>-3.3290528914343184E-18</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ref="I33:J33" si="21">SUM(I19:I32)</f>
+        <f t="shared" ref="I33:J33" si="22">SUM(I19:I32)</f>
         <v>-3.1431946129999928E-17</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="21"/>
-        <v>-3.3777179285350784E-17</v>
+        <f t="shared" si="22"/>
+        <v>-1.097414554905826E-15</v>
       </c>
       <c r="K33" t="s">
         <v>9</v>
@@ -2747,15 +2747,15 @@
         <v>3.362782661492857E-18</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" ref="M33:O33" si="22">SUM(M19:M32)</f>
+        <f t="shared" ref="M33:O33" si="23">SUM(M19:M32)</f>
         <v>3.6558199251635516E-17</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.1111169407673429E-15</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.1482057434454298E-15</v>
       </c>
     </row>
@@ -2774,15 +2774,15 @@
         <v>1.1390878648319285</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" ref="H36:J36" si="23">SIGN(H33)*SQRT(C33/M33)</f>
+        <f t="shared" ref="H36:J36" si="24">SIGN(H33)*SQRT(C33/M33)</f>
         <v>-0.88247247801805062</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>-0.96377199581265838</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>-0.96246941474551395</v>
       </c>
       <c r="L36" s="1"/>
@@ -2796,16 +2796,26 @@
         <v>2.9082013447084433E-9</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" ref="H37:J37" si="24">SQRT(2*C33-2*ABS(H36)*H33/((14-2)+M33))</f>
+        <f t="shared" ref="H37:J37" si="25">SQRT(2*C33-2*ABS(H36)*H33/((14-2)+M33))</f>
         <v>7.578231283684057E-9</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.5488297043042445E-8</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="24"/>
-        <v>4.6181089220271792E-8</v>
+        <f>2*E33-2*ABS(J36)*J33</f>
+        <v>4.2397306400277875E-15</v>
+      </c>
+      <c r="K37" s="1">
+        <f>J37/J38</f>
+        <v>0.30770694946081667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="J38" s="1">
+        <f>((14-2)*O33)</f>
+        <v>1.3778468921345158E-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>